<commit_message>
Remove solder paste from Tag Connect footprint
</commit_message>
<xml_diff>
--- a/x-IMU3-Thermometer-PCB/Project Outputs for x-IMU3-Thermometer/BOM/Bill of Materials-x-IMU3-Thermometer.xlsx
+++ b/x-IMU3-Thermometer-PCB/Project Outputs for x-IMU3-Thermometer/BOM/Bill of Materials-x-IMU3-Thermometer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\x-io\Products\x-IMU3\x-IMU3-Thermometer\x-IMU3-Thermometer-PCB\Project Outputs for x-IMU3-Thermometer\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF5C8789-9F69-4884-B514-C7C0947B7BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{197A4CD1-962A-4002-8B2E-77916D67E7C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35680" yWindow="3430" windowWidth="15060" windowHeight="13190" xr2:uid="{A1A12005-6301-4F3B-9369-EBBD5941A544}"/>
+    <workbookView xWindow="-24910" yWindow="2370" windowWidth="24840" windowHeight="19140" xr2:uid="{A5411F50-D2B3-4B3D-AC20-F081BA6610B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-x-IMU3-Thermo" sheetId="1" r:id="rId1"/>
@@ -514,7 +514,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AD9FC55-E8BB-4F04-B1B1-9F7040BD8CEF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2498308-CD39-43D8-95DE-157F83DA8068}">
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>